<commit_message>
more edits to taxon lists
</commit_message>
<xml_diff>
--- a/Data/taxa/Martone_Hakai_uniqueTaxa.xlsx
+++ b/Data/taxa/Martone_Hakai_uniqueTaxa.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\Martone Lab\martone_calvert\Data\taxa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F272E214-7C17-42C5-83BC-B7AE1A98EB6B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94970FF5-6287-4396-BCBE-5B6C56DF41C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="465" windowWidth="25365" windowHeight="14505" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="465" windowWidth="25365" windowHeight="14505" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General notes" sheetId="1" r:id="rId1"/>
@@ -1755,7 +1755,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2187,7 +2187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G464"/>
   <sheetViews>
     <sheetView zoomScale="134" workbookViewId="0"/>
@@ -5855,12 +5855,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B323" zoomScale="86" workbookViewId="0">
-      <selection activeCell="F345" sqref="F345"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6564,7 +6562,7 @@
         <v>90</v>
       </c>
       <c r="B44" t="str">
-        <f>A44</f>
+        <f t="shared" ref="B44:B50" si="3">A44</f>
         <v>Calliarthron tuberculosum</v>
       </c>
       <c r="D44" t="s">
@@ -6579,7 +6577,7 @@
         <v>92</v>
       </c>
       <c r="B45" t="str">
-        <f>A45</f>
+        <f t="shared" si="3"/>
         <v>Callithamnion pikeanum</v>
       </c>
       <c r="D45" t="s">
@@ -6594,7 +6592,7 @@
         <v>93</v>
       </c>
       <c r="B46" t="str">
-        <f>A46</f>
+        <f t="shared" si="3"/>
         <v>Callophyllis sp.</v>
       </c>
       <c r="D46" t="s">
@@ -6609,7 +6607,7 @@
         <v>94</v>
       </c>
       <c r="B47" t="str">
-        <f>A47</f>
+        <f t="shared" si="3"/>
         <v>Ceramium codicola</v>
       </c>
       <c r="D47" t="s">
@@ -6624,7 +6622,7 @@
         <v>95</v>
       </c>
       <c r="B48" t="str">
-        <f>A48</f>
+        <f t="shared" si="3"/>
         <v>Ceramium pacificum</v>
       </c>
       <c r="D48" t="s">
@@ -6639,7 +6637,7 @@
         <v>98</v>
       </c>
       <c r="B49" t="str">
-        <f>A49</f>
+        <f t="shared" si="3"/>
         <v>Chaetomorpha cannabina</v>
       </c>
       <c r="D49" t="s">
@@ -6654,7 +6652,7 @@
         <v>99</v>
       </c>
       <c r="B50" t="str">
-        <f>A50</f>
+        <f t="shared" si="3"/>
         <v>Chiharaea bodegensis</v>
       </c>
       <c r="D50" t="s">
@@ -6669,7 +6667,7 @@
         <v>100</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" ref="B51:B55" si="3">A51</f>
+        <f t="shared" ref="B51:B55" si="4">A51</f>
         <v>Chiharaea rhododactyla</v>
       </c>
       <c r="D51" t="s">
@@ -6684,7 +6682,7 @@
         <v>101</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Chiharaea silvae</v>
       </c>
       <c r="D52" t="s">
@@ -6699,7 +6697,7 @@
         <v>110</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Cladophora columbiana</v>
       </c>
       <c r="D53" t="s">
@@ -6714,7 +6712,7 @@
         <v>111</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Cladophora sericea</v>
       </c>
       <c r="D54" t="s">
@@ -6729,7 +6727,7 @@
         <v>112</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Cladophora stimpsonii</v>
       </c>
       <c r="D55" t="s">
@@ -6795,7 +6793,7 @@
         <v>120</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" ref="B59" si="4">A59</f>
+        <f t="shared" ref="B59" si="5">A59</f>
         <v>Codium fragile</v>
       </c>
       <c r="D59" t="s">
@@ -6885,7 +6883,7 @@
         <v>126</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" ref="B65:B66" si="5">A65</f>
+        <f t="shared" ref="B65:B66" si="6">A65</f>
         <v>Colpomenia peregrina</v>
       </c>
       <c r="D65" t="s">
@@ -6900,7 +6898,7 @@
         <v>127</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Constantinea subulifera</v>
       </c>
       <c r="D66" t="s">
@@ -6947,7 +6945,7 @@
         <v>131</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" ref="B69:B73" si="6">A69</f>
+        <f t="shared" ref="B69:B73" si="7">A69</f>
         <v>Corallina crust, unknown</v>
       </c>
       <c r="D69" t="s">
@@ -6962,7 +6960,7 @@
         <v>132</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Corallina frondescens</v>
       </c>
       <c r="D70" t="s">
@@ -6977,7 +6975,7 @@
         <v>133</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Corallina officianalis</v>
       </c>
       <c r="D71" t="s">
@@ -6992,7 +6990,7 @@
         <v>134</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Corallina officinalis</v>
       </c>
       <c r="D72" t="s">
@@ -7007,7 +7005,7 @@
         <v>129</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Corallina sp.</v>
       </c>
       <c r="D73" t="s">
@@ -7205,7 +7203,7 @@
         <v>150</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" ref="B86:B87" si="7">A86</f>
+        <f t="shared" ref="B86:B87" si="8">A86</f>
         <v>Cryptosiphonia woodii</v>
       </c>
       <c r="D86" t="s">
@@ -7220,7 +7218,7 @@
         <v>151</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Cumathamnion decipiens</v>
       </c>
       <c r="D87" t="s">
@@ -7351,7 +7349,7 @@
         <v>160</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" ref="B95:B100" si="8">A95</f>
+        <f t="shared" ref="B95:B100" si="9">A95</f>
         <v>Dilsea californica</v>
       </c>
       <c r="D95" t="s">
@@ -7366,7 +7364,7 @@
         <v>161</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Ectocarpus</v>
       </c>
       <c r="D96" t="s">
@@ -7381,7 +7379,7 @@
         <v>162</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Ectocarpus commensalis</v>
       </c>
       <c r="D97" t="s">
@@ -7396,7 +7394,7 @@
         <v>163</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Ectocarpus siliculosus</v>
       </c>
       <c r="D98" t="s">
@@ -7411,7 +7409,7 @@
         <v>164</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Egregia menziesii</v>
       </c>
       <c r="D99" t="s">
@@ -7426,7 +7424,7 @@
         <v>165</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Elachista fucicola</v>
       </c>
       <c r="D100" t="s">
@@ -7492,7 +7490,7 @@
         <v>171</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" ref="B104:B110" si="9">A104</f>
+        <f t="shared" ref="B104:B110" si="10">A104</f>
         <v>Endocladia muricata</v>
       </c>
       <c r="D104" t="s">
@@ -7507,7 +7505,7 @@
         <v>173</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Erythrotrichia carnea</v>
       </c>
       <c r="D105" t="s">
@@ -7522,7 +7520,7 @@
         <v>174</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Farlowia mollis</v>
       </c>
       <c r="D106" t="s">
@@ -7537,7 +7535,7 @@
         <v>175</v>
       </c>
       <c r="B107" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Fauchea sp.</v>
       </c>
       <c r="D107" t="s">
@@ -7555,7 +7553,7 @@
         <v>177</v>
       </c>
       <c r="B108" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Feldmannia irregularis</v>
       </c>
       <c r="D108" t="s">
@@ -7570,7 +7568,7 @@
         <v>182</v>
       </c>
       <c r="B109" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Frederikia sp.</v>
       </c>
       <c r="D109" s="7" t="s">
@@ -7585,7 +7583,7 @@
         <v>183</v>
       </c>
       <c r="B110" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Fucus distichus</v>
       </c>
       <c r="D110" t="s">
@@ -7617,7 +7615,7 @@
         <v>186</v>
       </c>
       <c r="B112" t="str">
-        <f t="shared" ref="B112:B116" si="10">A112</f>
+        <f t="shared" ref="B112:B116" si="11">A112</f>
         <v>Gelidium sp.</v>
       </c>
       <c r="D112" t="s">
@@ -7632,7 +7630,7 @@
         <v>187</v>
       </c>
       <c r="B113" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Gloiopeltis furcata</v>
       </c>
       <c r="D113" t="s">
@@ -7647,7 +7645,7 @@
         <v>191</v>
       </c>
       <c r="B114" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Gracilaria pacifica</v>
       </c>
       <c r="D114" t="s">
@@ -7662,7 +7660,7 @@
         <v>196</v>
       </c>
       <c r="B115" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Halosaccion glandiforme</v>
       </c>
       <c r="D115" t="s">
@@ -7677,7 +7675,7 @@
         <v>202</v>
       </c>
       <c r="B116" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Herposiphonia plumula</v>
       </c>
       <c r="D116" t="s">
@@ -7898,7 +7896,7 @@
         <v>225</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" ref="B130:B134" si="11">A130</f>
+        <f t="shared" ref="B130:B134" si="12">A130</f>
         <v>Kornmannia leptoderma</v>
       </c>
       <c r="D130" t="s">
@@ -7913,7 +7911,7 @@
         <v>227</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Laminaria setchellii</v>
       </c>
       <c r="D131" t="s">
@@ -7928,7 +7926,7 @@
         <v>228</v>
       </c>
       <c r="B132" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Laminaria yezoensis</v>
       </c>
       <c r="D132" t="s">
@@ -7943,7 +7941,7 @@
         <v>229</v>
       </c>
       <c r="B133" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Leathesia marina</v>
       </c>
       <c r="D133" t="s">
@@ -7961,7 +7959,7 @@
         <v>232</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Leptofauchea sp.</v>
       </c>
       <c r="D134" t="s">
@@ -8156,7 +8154,7 @@
         <v>251</v>
       </c>
       <c r="B146" t="str">
-        <f t="shared" ref="B146:B153" si="12">A146</f>
+        <f t="shared" ref="B146:B153" si="13">A146</f>
         <v>Lomentaria hakodatensis</v>
       </c>
       <c r="D146" t="s">
@@ -8171,7 +8169,7 @@
         <v>255</v>
       </c>
       <c r="B147" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Macrocystis pyrifera</v>
       </c>
       <c r="D147" t="s">
@@ -8186,7 +8184,7 @@
         <v>257</v>
       </c>
       <c r="B148" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Mastocarpus agardhii</v>
       </c>
       <c r="D148" t="s">
@@ -8201,7 +8199,7 @@
         <v>258</v>
       </c>
       <c r="B149" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Mastocarpus alaskensis</v>
       </c>
       <c r="D149" t="s">
@@ -8216,7 +8214,7 @@
         <v>259</v>
       </c>
       <c r="B150" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Mastocarpus intermedius</v>
       </c>
       <c r="D150" t="s">
@@ -8231,7 +8229,7 @@
         <v>260</v>
       </c>
       <c r="B151" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Mastocarpus latissimus</v>
       </c>
       <c r="D151" t="s">
@@ -8246,7 +8244,7 @@
         <v>261</v>
       </c>
       <c r="B152" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Mastocarpus pachenicus</v>
       </c>
       <c r="D152" t="s">
@@ -8261,7 +8259,7 @@
         <v>262</v>
       </c>
       <c r="B153" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Mastocarpus rigidus</v>
       </c>
       <c r="D153" t="s">
@@ -8513,7 +8511,7 @@
         <v>282</v>
       </c>
       <c r="B169" t="str">
-        <f t="shared" ref="B169:B171" si="13">A169</f>
+        <f t="shared" ref="B169:B171" si="14">A169</f>
         <v>Mesophyllum vancouveriense</v>
       </c>
       <c r="D169" t="s">
@@ -8528,7 +8526,7 @@
         <v>283</v>
       </c>
       <c r="B170" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Microcladia borealis</v>
       </c>
       <c r="D170" t="s">
@@ -8543,7 +8541,7 @@
         <v>284</v>
       </c>
       <c r="B171" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Monostroma grevillei</v>
       </c>
       <c r="D171" t="s">
@@ -8626,7 +8624,7 @@
         <v>298</v>
       </c>
       <c r="B176" t="str">
-        <f t="shared" ref="B176:B179" si="14">A176</f>
+        <f t="shared" ref="B176:B179" si="15">A176</f>
         <v>Neogastroclonium subarticulatum</v>
       </c>
       <c r="D176" t="s">
@@ -8641,7 +8639,7 @@
         <v>117</v>
       </c>
       <c r="B177" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Neopolyporolithon reclinatum</v>
       </c>
       <c r="C177" t="s">
@@ -8659,7 +8657,7 @@
         <v>300</v>
       </c>
       <c r="B178" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Neorhodomela aculeata</v>
       </c>
       <c r="D178" t="s">
@@ -8674,7 +8672,7 @@
         <v>301</v>
       </c>
       <c r="B179" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Neorhodomela larix</v>
       </c>
       <c r="D179" t="s">
@@ -8786,7 +8784,7 @@
         <v>314</v>
       </c>
       <c r="B186" t="str">
-        <f t="shared" ref="B186:B191" si="15">A186</f>
+        <f t="shared" ref="B186:B191" si="16">A186</f>
         <v>Odonthalia floccosa</v>
       </c>
       <c r="D186" t="s">
@@ -8801,7 +8799,7 @@
         <v>315</v>
       </c>
       <c r="B187" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Odonthalia floccosa f. comosa</v>
       </c>
       <c r="C187" t="s">
@@ -8819,7 +8817,7 @@
         <v>319</v>
       </c>
       <c r="B188" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Opuntiella californica</v>
       </c>
       <c r="D188" t="s">
@@ -8834,7 +8832,7 @@
         <v>324</v>
       </c>
       <c r="B189" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Osmundea spectabilis</v>
       </c>
       <c r="D189" t="s">
@@ -8849,7 +8847,7 @@
         <v>330</v>
       </c>
       <c r="B190" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Palmaria hecatensis</v>
       </c>
       <c r="D190" t="s">
@@ -8864,7 +8862,7 @@
         <v>331</v>
       </c>
       <c r="B191" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Palmaria mollis</v>
       </c>
       <c r="D191" t="s">
@@ -9044,7 +9042,7 @@
         <v>346</v>
       </c>
       <c r="B202" t="str">
-        <f t="shared" ref="B202:B206" si="16">A202</f>
+        <f t="shared" ref="B202:B206" si="17">A202</f>
         <v>Phyllospadix scouleri</v>
       </c>
       <c r="D202" t="s">
@@ -9059,7 +9057,7 @@
         <v>347</v>
       </c>
       <c r="B203" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Phyllospadix serrulatus</v>
       </c>
       <c r="D203" t="s">
@@ -9074,7 +9072,7 @@
         <v>353</v>
       </c>
       <c r="B204" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Pleonosporium vancouverianum</v>
       </c>
       <c r="D204" t="s">
@@ -9092,7 +9090,7 @@
         <v>354</v>
       </c>
       <c r="B205" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Plocamium pacificum</v>
       </c>
       <c r="D205" t="s">
@@ -9107,7 +9105,7 @@
         <v>355</v>
       </c>
       <c r="B206" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Plocamium violaceum</v>
       </c>
       <c r="D206" t="s">
@@ -9637,7 +9635,7 @@
         <v>393</v>
       </c>
       <c r="B237" t="str">
-        <f t="shared" ref="B237:B240" si="17">A237</f>
+        <f t="shared" ref="B237:B240" si="18">A237</f>
         <v>Pterosiphonia bipinnata</v>
       </c>
       <c r="D237" t="s">
@@ -9652,7 +9650,7 @@
         <v>394</v>
       </c>
       <c r="B238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Pterosiphonia dendroidea</v>
       </c>
       <c r="D238" t="s">
@@ -9667,7 +9665,7 @@
         <v>395</v>
       </c>
       <c r="B239" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Pterosiphonia gracilis</v>
       </c>
       <c r="D239" t="s">
@@ -9682,7 +9680,7 @@
         <v>396</v>
       </c>
       <c r="B240" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Pterygophora californica</v>
       </c>
       <c r="D240" t="s">
@@ -9728,7 +9726,7 @@
         <v>400</v>
       </c>
       <c r="B243" t="str">
-        <f t="shared" ref="B243:B246" si="18">A243</f>
+        <f t="shared" ref="B243:B246" si="19">A243</f>
         <v>Ptilota sp.</v>
       </c>
       <c r="D243" t="s">
@@ -9743,7 +9741,7 @@
         <v>401</v>
       </c>
       <c r="B244" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>Ptilota spp.</v>
       </c>
       <c r="D244" t="s">
@@ -9758,7 +9756,7 @@
         <v>402</v>
       </c>
       <c r="B245" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>Ptilota tenuis</v>
       </c>
       <c r="D245" t="s">
@@ -9773,7 +9771,7 @@
         <v>403</v>
       </c>
       <c r="B246" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>Pugetia firma</v>
       </c>
       <c r="D246" t="s">
@@ -9825,7 +9823,7 @@
         <v>410</v>
       </c>
       <c r="B249" t="str">
-        <f t="shared" ref="B249:B258" si="19">A249</f>
+        <f t="shared" ref="B249:B258" si="20">A249</f>
         <v>Punctaria sp.</v>
       </c>
       <c r="D249" t="s">
@@ -9843,7 +9841,7 @@
         <v>415</v>
       </c>
       <c r="B250" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pylaiella littoralis</v>
       </c>
       <c r="D250" t="s">
@@ -9858,7 +9856,7 @@
         <v>416</v>
       </c>
       <c r="B251" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pyropia abbottiae</v>
       </c>
       <c r="D251" t="s">
@@ -9873,7 +9871,7 @@
         <v>417</v>
       </c>
       <c r="B252" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pyropia fallax</v>
       </c>
       <c r="D252" t="s">
@@ -9888,7 +9886,7 @@
         <v>418</v>
       </c>
       <c r="B253" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pyropia fucicola</v>
       </c>
       <c r="D253" t="s">
@@ -9903,7 +9901,7 @@
         <v>419</v>
       </c>
       <c r="B254" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pyropia gardneri</v>
       </c>
       <c r="D254" t="s">
@@ -9918,7 +9916,7 @@
         <v>420</v>
       </c>
       <c r="B255" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pyropia perforata</v>
       </c>
       <c r="D255" t="s">
@@ -9933,7 +9931,7 @@
         <v>421</v>
       </c>
       <c r="B256" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pyropia schizophylla</v>
       </c>
       <c r="D256" t="s">
@@ -9948,7 +9946,7 @@
         <v>422</v>
       </c>
       <c r="B257" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pyropia smithii</v>
       </c>
       <c r="D257" t="s">
@@ -9963,7 +9961,7 @@
         <v>423</v>
       </c>
       <c r="B258" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Pyropia sp.</v>
       </c>
       <c r="D258" t="s">
@@ -10097,7 +10095,7 @@
         <v>432</v>
       </c>
       <c r="B266" t="str">
-        <f t="shared" ref="B266:B268" si="20">A266</f>
+        <f t="shared" ref="B266:B268" si="21">A266</f>
         <v>Red Crust</v>
       </c>
       <c r="C266" t="s">
@@ -10115,7 +10113,7 @@
         <v>435</v>
       </c>
       <c r="B267" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>Rhizoclonium tortuosum</v>
       </c>
       <c r="D267" t="s">
@@ -10130,7 +10128,7 @@
         <v>436</v>
       </c>
       <c r="B268" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>Rhodochorton purpureum</v>
       </c>
       <c r="D268" t="s">
@@ -10261,7 +10259,7 @@
         <v>446</v>
       </c>
       <c r="B276" t="str">
-        <f t="shared" ref="B276:B281" si="21">A276</f>
+        <f t="shared" ref="B276:B281" si="22">A276</f>
         <v>Salishia firma</v>
       </c>
       <c r="D276" t="s">
@@ -10279,7 +10277,7 @@
         <v>449</v>
       </c>
       <c r="B277" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Sargassum muticum</v>
       </c>
       <c r="D277" t="s">
@@ -10294,7 +10292,7 @@
         <v>450</v>
       </c>
       <c r="B278" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Scagelia occidentale</v>
       </c>
       <c r="D278" t="s">
@@ -10309,7 +10307,7 @@
         <v>451</v>
       </c>
       <c r="B279" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Schizymenia pacifica</v>
       </c>
       <c r="D279" t="s">
@@ -10324,7 +10322,7 @@
         <v>453</v>
       </c>
       <c r="B280" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Scytosiphon dotyi</v>
       </c>
       <c r="D280" t="s">
@@ -10339,7 +10337,7 @@
         <v>454</v>
       </c>
       <c r="B281" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Scytosiphon lomentaria</v>
       </c>
       <c r="D281" t="s">
@@ -10371,7 +10369,7 @@
         <v>461</v>
       </c>
       <c r="B283" t="str">
-        <f t="shared" ref="B283:B286" si="22">A283</f>
+        <f t="shared" ref="B283:B286" si="23">A283</f>
         <v>Smithora naiadum</v>
       </c>
       <c r="D283" t="s">
@@ -10386,7 +10384,7 @@
         <v>463</v>
       </c>
       <c r="B284" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Soranthera ulvoidea</v>
       </c>
       <c r="D284" t="s">
@@ -10404,7 +10402,7 @@
         <v>464</v>
       </c>
       <c r="B285" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Sparlingia pertusa</v>
       </c>
       <c r="D285" t="s">
@@ -10419,7 +10417,7 @@
         <v>465</v>
       </c>
       <c r="B286" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Sphacelaria rigidula</v>
       </c>
       <c r="D286" t="s">
@@ -10451,7 +10449,7 @@
         <v>478</v>
       </c>
       <c r="B288" t="str">
-        <f t="shared" ref="B288:B301" si="23">A288</f>
+        <f t="shared" ref="B288:B296" si="24">A288</f>
         <v>Tiffaniella snyderae</v>
       </c>
       <c r="D288" t="s">
@@ -10466,7 +10464,7 @@
         <v>479</v>
       </c>
       <c r="B289" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Tokidadendron bullatum</v>
       </c>
       <c r="D289" t="s">
@@ -10481,7 +10479,7 @@
         <v>487</v>
       </c>
       <c r="B290" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Ulothrix/Urospora</v>
       </c>
       <c r="D290" t="s">
@@ -10496,7 +10494,7 @@
         <v>488</v>
       </c>
       <c r="B291" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Ulva intestinalis</v>
       </c>
       <c r="D291" t="s">
@@ -10511,7 +10509,7 @@
         <v>489</v>
       </c>
       <c r="B292" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Ulva lactuca</v>
       </c>
       <c r="D292" t="s">
@@ -10526,7 +10524,7 @@
         <v>490</v>
       </c>
       <c r="B293" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Ulva linza</v>
       </c>
       <c r="D293" t="s">
@@ -10541,7 +10539,7 @@
         <v>491</v>
       </c>
       <c r="B294" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Ulva lobata</v>
       </c>
       <c r="D294" t="s">
@@ -10556,7 +10554,7 @@
         <v>492</v>
       </c>
       <c r="B295" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Ulva prolifera</v>
       </c>
       <c r="D295" t="s">
@@ -10571,7 +10569,7 @@
         <v>493</v>
       </c>
       <c r="B296" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Ulva sp.</v>
       </c>
       <c r="D296" t="s">
@@ -10739,7 +10737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>